<commit_message>
Adding covid images from both test and train sets; missed due to human error
</commit_message>
<xml_diff>
--- a/connect_core_data_set_xls.xlsx
+++ b/connect_core_data_set_xls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesdemott/Desktop/Bootcamp/UCB_COVID_Prediction_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12A20FD0-ADFB-274C-A656-402683EC667B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3FF224-4A30-8C43-B362-258D05FCD294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41780" yWindow="-3100" windowWidth="25420" windowHeight="21100" xr2:uid="{A41C7161-AFDF-9940-8B7A-EB7EF06FEE75}"/>
+    <workbookView xWindow="14820" yWindow="500" windowWidth="13980" windowHeight="17500" xr2:uid="{A41C7161-AFDF-9940-8B7A-EB7EF06FEE75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18003" uniqueCount="3018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18555" uniqueCount="3203">
   <si>
     <t>patient02332-study2-view1_frontal.jpg</t>
   </si>
@@ -9088,6 +9088,561 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>03BF7561-A9BA-4C3C-B8A0-D3E585F73F3C.jpeg</t>
+  </si>
+  <si>
+    <t>1-s2.0-S0140673620303706-fx1_lrg.jpg</t>
+  </si>
+  <si>
+    <t>1-s2.0-S0929664620300449-gr2_lrg-a.jpg</t>
+  </si>
+  <si>
+    <t>1-s2.0-S0929664620300449-gr2_lrg-b.jpg</t>
+  </si>
+  <si>
+    <t>1-s2.0-S0929664620300449-gr2_lrg-c.jpg</t>
+  </si>
+  <si>
+    <t>1-s2.0-S0929664620300449-gr2_lrg-d.jpg</t>
+  </si>
+  <si>
+    <t>1-s2.0-S1684118220300682-main.pdf-003-b1.png</t>
+  </si>
+  <si>
+    <t>1-s2.0-S1684118220300682-main.pdf-003-b2.png</t>
+  </si>
+  <si>
+    <t>1.CXRCTThoraximagesofCOVID-19fromSingapore.pdf-000-fig1a.png</t>
+  </si>
+  <si>
+    <t>1.CXRCTThoraximagesofCOVID-19fromSingapore.pdf-001-fig2b.png</t>
+  </si>
+  <si>
+    <t>1.CXRCTThoraximagesofCOVID-19fromSingapore.pdf-002-fig3a.png</t>
+  </si>
+  <si>
+    <t>1.CXRCTThoraximagesofCOVID-19fromSingapore.pdf-002-fig3b.png</t>
+  </si>
+  <si>
+    <t>1.CXRCTThoraximagesofCOVID-19fromSingapore.pdf-003-fig4a.png</t>
+  </si>
+  <si>
+    <t>1.CXRCTThoraximagesofCOVID-19fromSingapore.pdf-003-fig4b.png</t>
+  </si>
+  <si>
+    <t>1312A392-67A3-4EBF-9319-810CF6DA5EF6.jpeg</t>
+  </si>
+  <si>
+    <t>16654_1_1.png</t>
+  </si>
+  <si>
+    <t>16654_2_1.jpg</t>
+  </si>
+  <si>
+    <t>16654_4_1.jpg</t>
+  </si>
+  <si>
+    <t>16660_1_1.jpg</t>
+  </si>
+  <si>
+    <t>16660_2_1.jpg</t>
+  </si>
+  <si>
+    <t>16660_3_1.jpg</t>
+  </si>
+  <si>
+    <t>16660_4_1.jpg</t>
+  </si>
+  <si>
+    <t>16663_1_1.jpg</t>
+  </si>
+  <si>
+    <t>16669_1_1.jpeg</t>
+  </si>
+  <si>
+    <t>16669_3_1.jpeg</t>
+  </si>
+  <si>
+    <t>16672_1_1.jpg</t>
+  </si>
+  <si>
+    <t>16674_1_1.jpg</t>
+  </si>
+  <si>
+    <t>41591_2020_819_Fig1_HTML.webp-day10.png</t>
+  </si>
+  <si>
+    <t>41591_2020_819_Fig1_HTML.webp-day5.png</t>
+  </si>
+  <si>
+    <t>446B2CB6-B572-40AB-B01F-1910CA07086A.jpeg</t>
+  </si>
+  <si>
+    <t>4ad30bc6-2da0-4f84-bc9b-62acabfd518a.annot.original.png</t>
+  </si>
+  <si>
+    <t>53EC07C9-5CC6-4BE4-9B6F-D7B0D72AAA7E.jpeg</t>
+  </si>
+  <si>
+    <t>58cb9263f16e94305c730685358e4e_jumbo.jpeg</t>
+  </si>
+  <si>
+    <t>5CBC2E94-D358-401E-8928-965CCD965C5C.jpeg</t>
+  </si>
+  <si>
+    <t>6C94A287-C059-46A0-8600-AFB95F4727B7.jpeg</t>
+  </si>
+  <si>
+    <t>6b3bdbc31f65230b8cdcc3cef5f8ba8a-40ac-0.jpg</t>
+  </si>
+  <si>
+    <t>6b44464d-73a7-4cf3-bbb6-ffe7168300e3.annot.original.jpeg</t>
+  </si>
+  <si>
+    <t>7-fatal-covid19.jpg</t>
+  </si>
+  <si>
+    <t>7AF6C1AF-D249-4BD2-8C26-449304105D03.jpeg</t>
+  </si>
+  <si>
+    <t>88de9d8c39e946abd495b37cd07d89e5-0666-0.jpg</t>
+  </si>
+  <si>
+    <t>88de9d8c39e946abd495b37cd07d89e5-2ee6-0.jpg</t>
+  </si>
+  <si>
+    <t>88de9d8c39e946abd495b37cd07d89e5-6531-0.jpg</t>
+  </si>
+  <si>
+    <t>9fdd3c3032296fd04d2cad5d9070d4_jumbo.jpeg</t>
+  </si>
+  <si>
+    <t>A7E260CE-8A00-4C5F-A7F5-27336527A981.jpeg</t>
+  </si>
+  <si>
+    <t>AR-1.jpg</t>
+  </si>
+  <si>
+    <t>AR-2.jpg</t>
+  </si>
+  <si>
+    <t>B2D20576-00B7-4519-A415-72DE29C90C34.jpeg</t>
+  </si>
+  <si>
+    <t>CD50BA96-6982-4C80-AE7B-5F67ACDBFA56.jpeg</t>
+  </si>
+  <si>
+    <t>D7AF463C-2369-492D-908D-BE1911CCD74C.jpeg</t>
+  </si>
+  <si>
+    <t>E1724330-1866-4581-8CD8-CEC9B8AFEDDE.jpeg</t>
+  </si>
+  <si>
+    <t>F63AB6CE-1968-4154-A70F-913AF154F53D.jpeg</t>
+  </si>
+  <si>
+    <t>ajr.20.23034.pdf-001.png</t>
+  </si>
+  <si>
+    <t>ajr.20.23034.pdf-003.png</t>
+  </si>
+  <si>
+    <t>auntminnie-a-2020_01_28_23_51_6665_2020_01_28_Vietnam_coronavirus.jpeg</t>
+  </si>
+  <si>
+    <t>auntminnie-b-2020_01_28_23_51_6665_2020_01_28_Vietnam_coronavirus.jpeg</t>
+  </si>
+  <si>
+    <t>auntminnie-c-2020_01_28_23_51_6665_2020_01_28_Vietnam_coronavirus.jpeg</t>
+  </si>
+  <si>
+    <t>auntminnie-d-2020_01_28_23_51_6665_2020_01_28_Vietnam_coronavirus.jpeg</t>
+  </si>
+  <si>
+    <t>covid-19-infection-exclusive-gastrointestinal-symptoms-pa.png</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-12.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-14-PA.png</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-20-pa-on-admission.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-20.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-23-day1.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-23-day3.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-23-day9.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-24-day12.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-24-day6.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-24-day7.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-28.png</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-30-PA.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-42.jpeg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-49-day4.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-49-day8.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-58-day-10.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-58-day-7.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-58-day-9.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-67.jpeg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-bilateral.jpg</t>
+  </si>
+  <si>
+    <t>da9e9aac-de8c-44c7-ba57-e7cc8e4caaba.annot.original.jpeg</t>
+  </si>
+  <si>
+    <t>fff49165-b22d-4bb4-b9d1-d5d62c52436c.annot.original.png</t>
+  </si>
+  <si>
+    <t>figure1-5e73d7ae897e27ff066a30cb-98.jpeg</t>
+  </si>
+  <si>
+    <t>jkms-35-e79-g001-l-b.jpg</t>
+  </si>
+  <si>
+    <t>jkms-35-e79-g001-l-c.jpg</t>
+  </si>
+  <si>
+    <t>kjr-21-e24-g003-l-a.jpg</t>
+  </si>
+  <si>
+    <t>nejmc2001573_f1a.jpeg</t>
+  </si>
+  <si>
+    <t>nejmc2001573_f1b.jpeg</t>
+  </si>
+  <si>
+    <t>post-intubuation-pneumomediastium-and-pneumothorax-background-covid-19-pneumonia-day1.jpg</t>
+  </si>
+  <si>
+    <t>post-intubuation-pneumomediastium-and-pneumothorax-background-covid-19-pneumonia-day6-1.jpg</t>
+  </si>
+  <si>
+    <t>post-intubuation-pneumomediastium-and-pneumothorax-background-covid-19-pneumonia-day6-2.jpg</t>
+  </si>
+  <si>
+    <t>post-intubuation-pneumomediastium-and-pneumothorax-background-covid-19-pneumonia-day7.jpg</t>
+  </si>
+  <si>
+    <t>radiol.2020200490.fig3.jpeg</t>
+  </si>
+  <si>
+    <t>radiol.2020201160.fig2a.jpeg</t>
+  </si>
+  <si>
+    <t>radiol.2020201160.fig2c.jpeg</t>
+  </si>
+  <si>
+    <t>ryct.2020200028.fig1a.jpeg</t>
+  </si>
+  <si>
+    <t>ryct.2020200034.fig5-day0.jpeg</t>
+  </si>
+  <si>
+    <t>ryct.2020200034.fig5-day4.jpeg</t>
+  </si>
+  <si>
+    <t>ryct.2020200034.fig5-day7.jpeg</t>
+  </si>
+  <si>
+    <t>yxppt-2020-02-19_00-51-27_287214-day10.jpg</t>
+  </si>
+  <si>
+    <t>yxppt-2020-02-19_00-51-27_287214-day12.jpg</t>
+  </si>
+  <si>
+    <t>yxppt-2020-02-19_00-51-27_287214-day8.jpg</t>
+  </si>
+  <si>
+    <t>Covid</t>
+  </si>
+  <si>
+    <t>01E392EE-69F9-4E33-BFCE-E5C968654078.jpeg</t>
+  </si>
+  <si>
+    <t>1-s2.0-S1684118220300608-main.pdf-001.jpg</t>
+  </si>
+  <si>
+    <t>1-s2.0-S1684118220300608-main.pdf-002.jpg</t>
+  </si>
+  <si>
+    <t>1-s2.0-S1684118220300682-main.pdf-002-a1.png</t>
+  </si>
+  <si>
+    <t>1-s2.0-S1684118220300682-main.pdf-002-a2.png</t>
+  </si>
+  <si>
+    <t>16664_1_1.jpg</t>
+  </si>
+  <si>
+    <t>16691_1_1.jpg</t>
+  </si>
+  <si>
+    <t>171CB377-62FF-4B76-906C-F3787A01CB2E.jpeg</t>
+  </si>
+  <si>
+    <t>1B734A89-A1BF-49A8-A1D3-66FAFA4FAC5D.jpeg</t>
+  </si>
+  <si>
+    <t>2-chest-filmc.jpg</t>
+  </si>
+  <si>
+    <t>23E99E2E-447C-46E5-8EB2-D35D12473C39.png</t>
+  </si>
+  <si>
+    <t>2966893D-5DDF-4B68-9E2B-4979D5956C8E.jpeg</t>
+  </si>
+  <si>
+    <t>2B8649B2-00C4-4233-85D5-1CE240CF233B.jpeg</t>
+  </si>
+  <si>
+    <t>2C10A413-AABE-4807-8CCE-6A2025594067.jpeg</t>
+  </si>
+  <si>
+    <t>2C26F453-AF3B-4517-BB9E-802CF2179543.jpeg</t>
+  </si>
+  <si>
+    <t>31BA3780-2323-493F-8AED-62081B9C383B.jpeg</t>
+  </si>
+  <si>
+    <t>353889E0-A1E8-4F9E-A0B8-F24F36BCFBFB.jpeg</t>
+  </si>
+  <si>
+    <t>39EE8E69-5801-48DE-B6E3-BE7D1BCF3092.jpeg</t>
+  </si>
+  <si>
+    <t>4-x-day1.jpg</t>
+  </si>
+  <si>
+    <t>4-x-day13.jpg</t>
+  </si>
+  <si>
+    <t>4-x-day4.jpg</t>
+  </si>
+  <si>
+    <t>4-x-day8.jpg</t>
+  </si>
+  <si>
+    <t>4e43e48d52c9e2d4c6c1fb9bc1544f_jumbo.jpeg</t>
+  </si>
+  <si>
+    <t>5931B64A-7B97-485D-BE60-3F1EA76BC4F0.jpeg</t>
+  </si>
+  <si>
+    <t>5A78BCA9-5B7A-440D-8A4E-AE7710EA6EAD.jpeg</t>
+  </si>
+  <si>
+    <t>5e6dd879fde9502400e58b2f.jpeg</t>
+  </si>
+  <si>
+    <t>67d668e570c242404ba82c7cbe2ca8f2-0015-0.jpg</t>
+  </si>
+  <si>
+    <t>67d668e570c242404ba82c7cbe2ca8f2-05be-0.jpg</t>
+  </si>
+  <si>
+    <t>6CB4EFC6-68FA-4CD5-940C-BEFA8DAFE9A7.jpeg</t>
+  </si>
+  <si>
+    <t>7E335538-2F86-424E-A0AB-6397783A38D0.jpeg</t>
+  </si>
+  <si>
+    <t>80446565-E090-4187-A031-9D3CEAA586C8.jpeg</t>
+  </si>
+  <si>
+    <t>85E52EB3-56E9-4D67-82DA-DEA247C82886.jpeg</t>
+  </si>
+  <si>
+    <t>8FDE8DBA-CFBD-4B4C-B1A4-6F36A93B7E87.jpeg</t>
+  </si>
+  <si>
+    <t>93FE0BB1-022D-4F24-9727-987A07975FFB.jpeg</t>
+  </si>
+  <si>
+    <t>9C34AF49-E589-44D5-92D3-168B3B04E4A6.jpeg</t>
+  </si>
+  <si>
+    <t>B59DD164-51D5-40DF-A926-6A42DD52EBE8.jpeg</t>
+  </si>
+  <si>
+    <t>C6EA0BE5-B01E-4113-B194-18D956675E25.jpeg</t>
+  </si>
+  <si>
+    <t>E63574A7-4188-4C8D-8D17-9D67A18A1AFA.jpeg</t>
+  </si>
+  <si>
+    <t>F2DE909F-E19C-4900-92F5-8F435B031AC6.jpeg</t>
+  </si>
+  <si>
+    <t>F4341CE7-73C9-45C6-99C8-8567A5484B63.jpeg</t>
+  </si>
+  <si>
+    <t>FE9F9A5D-2830-46F9-851B-1FF4534959BE.jpeg</t>
+  </si>
+  <si>
+    <t>RX-torace-a-letto-del-paziente-in-unica-proiezione-AP-1-1.jpeg</t>
+  </si>
+  <si>
+    <t>ae6c954c0039de4b5edee53865ffee43-e6c8-0.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-caso-70-1-PA.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-caso-70-2-APS.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-15-PA.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-2.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-22-day1-pa.png</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-22-day2-pa.png</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-34.png</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-35-1.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-35-2.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-40.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-41-day-0.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-41-day-2.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-43-day0.jpeg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-43-day2.jpeg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-7-PA.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-evolution-over-a-week-1-day0-PA.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-evolution-over-a-week-1-day3.jpg</t>
+  </si>
+  <si>
+    <t>covid-19-pneumonia-evolution-over-a-week-1-day4.jpg</t>
+  </si>
+  <si>
+    <t>extubation-1.jpg</t>
+  </si>
+  <si>
+    <t>extubation-13.jpg</t>
+  </si>
+  <si>
+    <t>extubation-4.jpg</t>
+  </si>
+  <si>
+    <t>extubation-8.jpg</t>
+  </si>
+  <si>
+    <t>figure1-5e71be566aa8714a04de3386-98-left.jpeg</t>
+  </si>
+  <si>
+    <t>figure1-5e75d0940b71e1b702629659-98-right.jpeg</t>
+  </si>
+  <si>
+    <t>figure1-5e7c1b8d98c29ab001275405-98-later.jpeg</t>
+  </si>
+  <si>
+    <t>figure1-5e7c1b8d98c29ab001275405-98.jpeg</t>
+  </si>
+  <si>
+    <t>gr1_lrg-a.jpg</t>
+  </si>
+  <si>
+    <t>kjr-21-e24-g001-l-a.jpg</t>
+  </si>
+  <si>
+    <t>kjr-21-e24-g002-l-a.jpg</t>
+  </si>
+  <si>
+    <t>lancet-case2a.jpg</t>
+  </si>
+  <si>
+    <t>lancet-case2b.jpg</t>
+  </si>
+  <si>
+    <t>nejmoa2001191_f3-PA.jpeg</t>
+  </si>
+  <si>
+    <t>nejmoa2001191_f4.jpeg</t>
+  </si>
+  <si>
+    <t>nejmoa2001191_f5-PA.jpeg</t>
+  </si>
+  <si>
+    <t>paving.jpg</t>
+  </si>
+  <si>
+    <t>radiol.2020201160.fig2b.jpeg</t>
+  </si>
+  <si>
+    <t>radiol.2020201160.fig2d.jpeg</t>
+  </si>
+  <si>
+    <t>radiol.2020201160.fig3a.jpeg</t>
+  </si>
+  <si>
+    <t>radiol.2020201160.fig3c.jpeg</t>
+  </si>
+  <si>
+    <t>radiol.2020201160.fig3d.jpeg</t>
+  </si>
+  <si>
+    <t>ryct.2020200034.fig2.jpeg</t>
   </si>
 </sst>
 </file>
@@ -9129,12 +9684,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9460,9 +10016,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D16FD4B-CF38-3B4C-B620-3CC280DEC34A}">
-  <dimension ref="A1:C6001"/>
+  <dimension ref="A1:C6185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -75480,9 +76038,2033 @@
         <v>3017</v>
       </c>
     </row>
+    <row r="6002" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6002" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6002" s="1" t="s">
+        <v>3018</v>
+      </c>
+      <c r="C6002" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6003" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6003" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6003" s="1" t="s">
+        <v>3019</v>
+      </c>
+      <c r="C6003" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6004" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6004" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6004" s="1" t="s">
+        <v>3020</v>
+      </c>
+      <c r="C6004" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6005" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6005" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6005" s="1" t="s">
+        <v>3021</v>
+      </c>
+      <c r="C6005" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6006" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6006" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6006" s="1" t="s">
+        <v>3022</v>
+      </c>
+      <c r="C6006" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6007" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6007" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6007" s="1" t="s">
+        <v>3023</v>
+      </c>
+      <c r="C6007" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6008" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6008" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6008" s="1" t="s">
+        <v>3024</v>
+      </c>
+      <c r="C6008" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6009" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6009" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6009" s="1" t="s">
+        <v>3025</v>
+      </c>
+      <c r="C6009" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6010" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6010" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6010" s="1" t="s">
+        <v>3026</v>
+      </c>
+      <c r="C6010" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6011" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6011" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6011" s="1" t="s">
+        <v>3027</v>
+      </c>
+      <c r="C6011" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6012" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6012" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6012" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="C6012" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6013" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6013" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6013" s="1" t="s">
+        <v>3029</v>
+      </c>
+      <c r="C6013" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6014" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6014" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6014" s="1" t="s">
+        <v>3030</v>
+      </c>
+      <c r="C6014" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6015" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6015" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6015" s="1" t="s">
+        <v>3031</v>
+      </c>
+      <c r="C6015" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6016" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6016" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6016" s="1" t="s">
+        <v>3032</v>
+      </c>
+      <c r="C6016" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6017" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6017" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6017" s="1" t="s">
+        <v>3033</v>
+      </c>
+      <c r="C6017" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6018" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6018" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6018" s="1" t="s">
+        <v>3034</v>
+      </c>
+      <c r="C6018" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6019" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6019" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6019" s="1" t="s">
+        <v>3035</v>
+      </c>
+      <c r="C6019" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6020" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6020" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6020" s="1" t="s">
+        <v>3036</v>
+      </c>
+      <c r="C6020" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6021" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6021" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6021" s="1" t="s">
+        <v>3037</v>
+      </c>
+      <c r="C6021" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6022" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6022" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6022" s="1" t="s">
+        <v>3038</v>
+      </c>
+      <c r="C6022" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6023" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6023" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6023" s="1" t="s">
+        <v>3039</v>
+      </c>
+      <c r="C6023" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6024" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6024" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6024" s="1" t="s">
+        <v>3040</v>
+      </c>
+      <c r="C6024" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6025" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6025" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6025" s="1" t="s">
+        <v>3041</v>
+      </c>
+      <c r="C6025" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6026" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6026" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6026" s="1" t="s">
+        <v>3042</v>
+      </c>
+      <c r="C6026" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6027" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6027" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6027" s="1" t="s">
+        <v>3043</v>
+      </c>
+      <c r="C6027" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6028" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6028" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6028" s="1" t="s">
+        <v>3044</v>
+      </c>
+      <c r="C6028" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6029" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6029" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6029" s="1" t="s">
+        <v>3045</v>
+      </c>
+      <c r="C6029" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6030" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6030" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6030" s="1" t="s">
+        <v>3046</v>
+      </c>
+      <c r="C6030" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6031" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6031" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6031" s="1" t="s">
+        <v>3047</v>
+      </c>
+      <c r="C6031" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6032" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6032" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6032" s="1" t="s">
+        <v>3048</v>
+      </c>
+      <c r="C6032" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6033" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6033" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6033" s="1" t="s">
+        <v>3049</v>
+      </c>
+      <c r="C6033" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6034" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6034" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6034" s="1" t="s">
+        <v>3050</v>
+      </c>
+      <c r="C6034" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6035" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6035" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6035" s="1" t="s">
+        <v>3051</v>
+      </c>
+      <c r="C6035" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6036" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6036" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6036" s="1" t="s">
+        <v>3052</v>
+      </c>
+      <c r="C6036" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6037" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6037" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6037" s="1" t="s">
+        <v>3053</v>
+      </c>
+      <c r="C6037" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6038" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6038" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6038" s="1" t="s">
+        <v>3054</v>
+      </c>
+      <c r="C6038" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6039" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6039" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6039" s="1" t="s">
+        <v>3055</v>
+      </c>
+      <c r="C6039" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6040" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6040" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6040" s="1" t="s">
+        <v>3056</v>
+      </c>
+      <c r="C6040" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6041" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6041" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6041" s="1" t="s">
+        <v>3057</v>
+      </c>
+      <c r="C6041" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6042" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6042" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6042" s="1" t="s">
+        <v>3058</v>
+      </c>
+      <c r="C6042" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6043" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6043" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6043" s="1" t="s">
+        <v>3059</v>
+      </c>
+      <c r="C6043" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6044" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6044" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6044" s="1" t="s">
+        <v>3060</v>
+      </c>
+      <c r="C6044" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6045" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6045" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6045" s="1" t="s">
+        <v>3061</v>
+      </c>
+      <c r="C6045" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6046" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6046" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6046" s="1" t="s">
+        <v>3062</v>
+      </c>
+      <c r="C6046" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6047" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6047" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6047" s="1" t="s">
+        <v>3063</v>
+      </c>
+      <c r="C6047" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6048" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6048" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6048" s="1" t="s">
+        <v>3064</v>
+      </c>
+      <c r="C6048" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6049" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6049" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6049" s="1" t="s">
+        <v>3065</v>
+      </c>
+      <c r="C6049" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6050" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6050" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6050" s="1" t="s">
+        <v>3066</v>
+      </c>
+      <c r="C6050" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6051" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6051" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6051" s="1" t="s">
+        <v>3067</v>
+      </c>
+      <c r="C6051" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6052" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6052" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6052" s="1" t="s">
+        <v>3068</v>
+      </c>
+      <c r="C6052" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6053" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6053" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6053" s="1" t="s">
+        <v>3069</v>
+      </c>
+      <c r="C6053" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6054" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6054" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6054" s="1" t="s">
+        <v>3070</v>
+      </c>
+      <c r="C6054" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6055" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6055" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6055" s="1" t="s">
+        <v>3071</v>
+      </c>
+      <c r="C6055" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6056" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6056" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6056" s="1" t="s">
+        <v>3072</v>
+      </c>
+      <c r="C6056" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6057" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6057" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6057" s="1" t="s">
+        <v>3073</v>
+      </c>
+      <c r="C6057" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6058" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6058" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6058" s="1" t="s">
+        <v>3074</v>
+      </c>
+      <c r="C6058" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6059" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6059" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6059" s="1" t="s">
+        <v>3075</v>
+      </c>
+      <c r="C6059" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6060" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6060" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6060" s="1" t="s">
+        <v>3076</v>
+      </c>
+      <c r="C6060" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6061" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6061" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6061" s="1" t="s">
+        <v>3077</v>
+      </c>
+      <c r="C6061" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6062" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6062" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6062" s="1" t="s">
+        <v>3078</v>
+      </c>
+      <c r="C6062" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6063" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6063" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6063" s="1" t="s">
+        <v>3079</v>
+      </c>
+      <c r="C6063" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6064" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6064" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6064" s="1" t="s">
+        <v>3080</v>
+      </c>
+      <c r="C6064" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6065" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6065" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6065" s="1" t="s">
+        <v>3081</v>
+      </c>
+      <c r="C6065" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6066" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6066" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6066" s="1" t="s">
+        <v>3082</v>
+      </c>
+      <c r="C6066" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6067" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6067" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6067" s="1" t="s">
+        <v>3083</v>
+      </c>
+      <c r="C6067" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6068" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6068" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6068" s="1" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C6068" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6069" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6069" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6069" s="1" t="s">
+        <v>3085</v>
+      </c>
+      <c r="C6069" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6070" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6070" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6070" s="1" t="s">
+        <v>3086</v>
+      </c>
+      <c r="C6070" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6071" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6071" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6071" s="1" t="s">
+        <v>3087</v>
+      </c>
+      <c r="C6071" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6072" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6072" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6072" s="1" t="s">
+        <v>3088</v>
+      </c>
+      <c r="C6072" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6073" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6073" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6073" s="1" t="s">
+        <v>3089</v>
+      </c>
+      <c r="C6073" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6074" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6074" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6074" s="1" t="s">
+        <v>3090</v>
+      </c>
+      <c r="C6074" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6075" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6075" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6075" s="1" t="s">
+        <v>3091</v>
+      </c>
+      <c r="C6075" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6076" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6076" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6076" s="1" t="s">
+        <v>3092</v>
+      </c>
+      <c r="C6076" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6077" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6077" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6077" s="1" t="s">
+        <v>3093</v>
+      </c>
+      <c r="C6077" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6078" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6078" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6078" s="1" t="s">
+        <v>3094</v>
+      </c>
+      <c r="C6078" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6079" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6079" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6079" s="1" t="s">
+        <v>3095</v>
+      </c>
+      <c r="C6079" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6080" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6080" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6080" s="1" t="s">
+        <v>3096</v>
+      </c>
+      <c r="C6080" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6081" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6081" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6081" s="1" t="s">
+        <v>3097</v>
+      </c>
+      <c r="C6081" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6082" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6082" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6082" s="1" t="s">
+        <v>3098</v>
+      </c>
+      <c r="C6082" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6083" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6083" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6083" s="1" t="s">
+        <v>3099</v>
+      </c>
+      <c r="C6083" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6084" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6084" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6084" s="1" t="s">
+        <v>3100</v>
+      </c>
+      <c r="C6084" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6085" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6085" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6085" s="1" t="s">
+        <v>3101</v>
+      </c>
+      <c r="C6085" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6086" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6086" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6086" s="1" t="s">
+        <v>3102</v>
+      </c>
+      <c r="C6086" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6087" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6087" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6087" s="1" t="s">
+        <v>3103</v>
+      </c>
+      <c r="C6087" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6088" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6088" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6088" s="1" t="s">
+        <v>3104</v>
+      </c>
+      <c r="C6088" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6089" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6089" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6089" s="1" t="s">
+        <v>3105</v>
+      </c>
+      <c r="C6089" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6090" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6090" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6090" s="1" t="s">
+        <v>3106</v>
+      </c>
+      <c r="C6090" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6091" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6091" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6091" s="1" t="s">
+        <v>3107</v>
+      </c>
+      <c r="C6091" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6092" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6092" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6092" s="1" t="s">
+        <v>3108</v>
+      </c>
+      <c r="C6092" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6093" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6093" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6093" s="1" t="s">
+        <v>3109</v>
+      </c>
+      <c r="C6093" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6094" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6094" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6094" s="1" t="s">
+        <v>3110</v>
+      </c>
+      <c r="C6094" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6095" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6095" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6095" s="1" t="s">
+        <v>3111</v>
+      </c>
+      <c r="C6095" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6096" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6096" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6096" s="1" t="s">
+        <v>3112</v>
+      </c>
+      <c r="C6096" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6097" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6097" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6097" s="1" t="s">
+        <v>3113</v>
+      </c>
+      <c r="C6097" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6098" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6098" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6098" s="1" t="s">
+        <v>3114</v>
+      </c>
+      <c r="C6098" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6099" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6099" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6099" s="1" t="s">
+        <v>3115</v>
+      </c>
+      <c r="C6099" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6100" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6100" s="1" t="s">
+        <v>3116</v>
+      </c>
+      <c r="C6100" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6101" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6101" s="1" t="s">
+        <v>3117</v>
+      </c>
+      <c r="C6101" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="6102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6102" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6102" s="3" t="s">
+        <v>3119</v>
+      </c>
+      <c r="C6102" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6103" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6103" s="1" t="s">
+        <v>3120</v>
+      </c>
+      <c r="C6103" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6104" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6104" s="1" t="s">
+        <v>3121</v>
+      </c>
+      <c r="C6104" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6105" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6105" s="1" t="s">
+        <v>3122</v>
+      </c>
+      <c r="C6105" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6106" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6106" s="1" t="s">
+        <v>3123</v>
+      </c>
+      <c r="C6106" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6107" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6107" s="1" t="s">
+        <v>3124</v>
+      </c>
+      <c r="C6107" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6108" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6108" s="1" t="s">
+        <v>3125</v>
+      </c>
+      <c r="C6108" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6109" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6109" s="1" t="s">
+        <v>3126</v>
+      </c>
+      <c r="C6109" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6110" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6110" s="1" t="s">
+        <v>3127</v>
+      </c>
+      <c r="C6110" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6111" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6111" s="1" t="s">
+        <v>3128</v>
+      </c>
+      <c r="C6111" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6112" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6112" s="1" t="s">
+        <v>3129</v>
+      </c>
+      <c r="C6112" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6113" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6113" s="1" t="s">
+        <v>3130</v>
+      </c>
+      <c r="C6113" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6114" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6114" s="1" t="s">
+        <v>3131</v>
+      </c>
+      <c r="C6114" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6115" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6115" s="1" t="s">
+        <v>3132</v>
+      </c>
+      <c r="C6115" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6116" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6116" s="1" t="s">
+        <v>3133</v>
+      </c>
+      <c r="C6116" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6117" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6117" s="1" t="s">
+        <v>3134</v>
+      </c>
+      <c r="C6117" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6118" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6118" s="1" t="s">
+        <v>3135</v>
+      </c>
+      <c r="C6118" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6119" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6119" s="1" t="s">
+        <v>3136</v>
+      </c>
+      <c r="C6119" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6120" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6120" s="1" t="s">
+        <v>3137</v>
+      </c>
+      <c r="C6120" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6121" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6121" s="1" t="s">
+        <v>3138</v>
+      </c>
+      <c r="C6121" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6122" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6122" s="1" t="s">
+        <v>3139</v>
+      </c>
+      <c r="C6122" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6123" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6123" s="1" t="s">
+        <v>3140</v>
+      </c>
+      <c r="C6123" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6124" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6124" s="1" t="s">
+        <v>3141</v>
+      </c>
+      <c r="C6124" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6125" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6125" s="1" t="s">
+        <v>3142</v>
+      </c>
+      <c r="C6125" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6126" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6126" s="1" t="s">
+        <v>3143</v>
+      </c>
+      <c r="C6126" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6127" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6127" s="1" t="s">
+        <v>3144</v>
+      </c>
+      <c r="C6127" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6128" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6128" s="1" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C6128" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6129" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6129" s="1" t="s">
+        <v>3146</v>
+      </c>
+      <c r="C6129" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6130" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6130" s="1" t="s">
+        <v>3147</v>
+      </c>
+      <c r="C6130" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6131" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6131" s="3" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C6131" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6132" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6132" s="1" t="s">
+        <v>3149</v>
+      </c>
+      <c r="C6132" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6133" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6133" s="1" t="s">
+        <v>3150</v>
+      </c>
+      <c r="C6133" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6134" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6134" s="1" t="s">
+        <v>3151</v>
+      </c>
+      <c r="C6134" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6135" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6135" s="1" t="s">
+        <v>3152</v>
+      </c>
+      <c r="C6135" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6136" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6136" s="1" t="s">
+        <v>3153</v>
+      </c>
+      <c r="C6136" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6137" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6137" s="1" t="s">
+        <v>3154</v>
+      </c>
+      <c r="C6137" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6138" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6138" s="1" t="s">
+        <v>3155</v>
+      </c>
+      <c r="C6138" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6139" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6139" s="1" t="s">
+        <v>3156</v>
+      </c>
+      <c r="C6139" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6140" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6140" s="1" t="s">
+        <v>3157</v>
+      </c>
+      <c r="C6140" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6141" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6141" s="1" t="s">
+        <v>3158</v>
+      </c>
+      <c r="C6141" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6142" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6142" s="1" t="s">
+        <v>3159</v>
+      </c>
+      <c r="C6142" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6143" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6143" s="1" t="s">
+        <v>3160</v>
+      </c>
+      <c r="C6143" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6144" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6144" s="1" t="s">
+        <v>3161</v>
+      </c>
+      <c r="C6144" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6145" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6145" s="1" t="s">
+        <v>3162</v>
+      </c>
+      <c r="C6145" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6146" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6146" s="1" t="s">
+        <v>3163</v>
+      </c>
+      <c r="C6146" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6147" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6147" s="1" t="s">
+        <v>3164</v>
+      </c>
+      <c r="C6147" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6148" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6148" s="1" t="s">
+        <v>3165</v>
+      </c>
+      <c r="C6148" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6149" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6149" s="1" t="s">
+        <v>3166</v>
+      </c>
+      <c r="C6149" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6150" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6150" s="1" t="s">
+        <v>3167</v>
+      </c>
+      <c r="C6150" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6151" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6151" s="1" t="s">
+        <v>3168</v>
+      </c>
+      <c r="C6151" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6152" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6152" s="1" t="s">
+        <v>3169</v>
+      </c>
+      <c r="C6152" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6153" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6153" s="1" t="s">
+        <v>3170</v>
+      </c>
+      <c r="C6153" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6154" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6154" s="1" t="s">
+        <v>3171</v>
+      </c>
+      <c r="C6154" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6155" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6155" s="1" t="s">
+        <v>3172</v>
+      </c>
+      <c r="C6155" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6156" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6156" s="1" t="s">
+        <v>3173</v>
+      </c>
+      <c r="C6156" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6157" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6157" s="1" t="s">
+        <v>3174</v>
+      </c>
+      <c r="C6157" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6158" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6158" s="1" t="s">
+        <v>3175</v>
+      </c>
+      <c r="C6158" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6159" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6159" s="1" t="s">
+        <v>3176</v>
+      </c>
+      <c r="C6159" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6160" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6160" s="1" t="s">
+        <v>3177</v>
+      </c>
+      <c r="C6160" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6161" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6161" s="1" t="s">
+        <v>3178</v>
+      </c>
+      <c r="C6161" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6162" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6162" s="1" t="s">
+        <v>3179</v>
+      </c>
+      <c r="C6162" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6163" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6163" s="1" t="s">
+        <v>3180</v>
+      </c>
+      <c r="C6163" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6164" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6164" s="1" t="s">
+        <v>3181</v>
+      </c>
+      <c r="C6164" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6165" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6165" s="1" t="s">
+        <v>3182</v>
+      </c>
+      <c r="C6165" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6166" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6166" s="1" t="s">
+        <v>3183</v>
+      </c>
+      <c r="C6166" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6167" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6167" s="1" t="s">
+        <v>3184</v>
+      </c>
+      <c r="C6167" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6168" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6168" s="1" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C6168" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6169" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6169" s="1" t="s">
+        <v>3186</v>
+      </c>
+      <c r="C6169" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6170" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6170" s="1" t="s">
+        <v>3187</v>
+      </c>
+      <c r="C6170" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6171" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6171" s="1" t="s">
+        <v>3188</v>
+      </c>
+      <c r="C6171" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6172" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6172" s="1" t="s">
+        <v>3189</v>
+      </c>
+      <c r="C6172" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6173" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6173" s="1" t="s">
+        <v>3190</v>
+      </c>
+      <c r="C6173" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6174" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6174" s="1" t="s">
+        <v>3191</v>
+      </c>
+      <c r="C6174" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6175" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6175" s="1" t="s">
+        <v>3192</v>
+      </c>
+      <c r="C6175" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6176" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6176" s="1" t="s">
+        <v>3193</v>
+      </c>
+      <c r="C6176" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6177" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6177" s="1" t="s">
+        <v>3194</v>
+      </c>
+      <c r="C6177" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6178" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6178" s="1" t="s">
+        <v>3195</v>
+      </c>
+      <c r="C6178" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6179" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6179" s="1" t="s">
+        <v>3196</v>
+      </c>
+      <c r="C6179" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6180" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6180" s="1" t="s">
+        <v>3197</v>
+      </c>
+      <c r="C6180" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6181" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6181" s="1" t="s">
+        <v>3198</v>
+      </c>
+      <c r="C6181" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6182" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6182" s="1" t="s">
+        <v>3199</v>
+      </c>
+      <c r="C6182" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6183" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6183" s="1" t="s">
+        <v>3200</v>
+      </c>
+      <c r="C6183" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6184" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6184" s="1" t="s">
+        <v>3201</v>
+      </c>
+      <c r="C6184" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="6185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6185" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B6185" s="1" t="s">
+        <v>3202</v>
+      </c>
+      <c r="C6185" t="s">
+        <v>3016</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="B6002:B1048576 B1:B3001">
+  <conditionalFormatting sqref="B6186:B1048576 B1:B3001">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>